<commit_message>
Add all changes including output directory
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-assistance-required.xlsx
+++ b/output/StructureDefinition-assistance-required.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-26T11:43:49-04:00</t>
+    <t>2022-05-13T16:07:55-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -666,42 +666,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.2890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="36.40625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="19.796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="27.6875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.44140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="26.53515625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.67578125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="22.671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>